<commit_message>
put older files into archive
</commit_message>
<xml_diff>
--- a/output_files/cl_3.xlsx
+++ b/output_files/cl_3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/galileo/development/Reserch/UMN_Research/CCDPA_git/CCDPApy/output_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADC65E63-A3D4-A640-AAE8-9DF6CF23858A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C227297B-A6E7-BF44-8F35-FABC2FEE3FE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="500" windowWidth="22360" windowHeight="13840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="240" yWindow="500" windowWidth="28420" windowHeight="16100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sample CL3_1" sheetId="1" r:id="rId1"/>
@@ -878,8 +878,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:FF16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" topLeftCell="EE1" zoomScale="133" workbookViewId="0">
+      <selection activeCell="EO19" sqref="EO19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1550,7 +1550,7 @@
         <v>2.5694444448163271E-2</v>
       </c>
       <c r="E2">
-        <v>0.61666666675591841</v>
+        <v>0.61666666675591797</v>
       </c>
       <c r="F2">
         <v>20</v>
@@ -4820,6 +4820,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -4827,9 +4828,174 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:FF16"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="EL1" workbookViewId="0">
+      <selection activeCell="EO21" sqref="EO21"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="30.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="29.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="29.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="3.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="42.33203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="21" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="18" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="16" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="24" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="16" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="20" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="22" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="19" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="20" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="22.5" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="25.5" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="19" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="21.1640625" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="23" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="25.1640625" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="22" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="25.1640625" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="24" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="21.1640625" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="24.5" bestFit="1" customWidth="1"/>
+    <col min="76" max="76" width="24.83203125" bestFit="1" customWidth="1"/>
+    <col min="77" max="77" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="78" max="78" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="79" max="79" width="24" bestFit="1" customWidth="1"/>
+    <col min="80" max="80" width="21.83203125" bestFit="1" customWidth="1"/>
+    <col min="81" max="81" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="82" max="82" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="83" max="83" width="25" bestFit="1" customWidth="1"/>
+    <col min="84" max="84" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="85" max="85" width="28.1640625" bestFit="1" customWidth="1"/>
+    <col min="86" max="86" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="87" max="87" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="88" max="88" width="23.83203125" bestFit="1" customWidth="1"/>
+    <col min="89" max="89" width="25.5" bestFit="1" customWidth="1"/>
+    <col min="90" max="90" width="22.5" bestFit="1" customWidth="1"/>
+    <col min="91" max="91" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="92" max="92" width="27.83203125" bestFit="1" customWidth="1"/>
+    <col min="93" max="93" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="94" max="94" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="95" max="95" width="20" bestFit="1" customWidth="1"/>
+    <col min="96" max="96" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="97" max="97" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="98" max="98" width="17" bestFit="1" customWidth="1"/>
+    <col min="99" max="99" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="100" max="100" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="101" max="101" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="102" max="102" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="103" max="103" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="104" max="104" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="105" max="105" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="106" max="106" width="15" bestFit="1" customWidth="1"/>
+    <col min="107" max="107" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="108" max="108" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="109" max="109" width="23" bestFit="1" customWidth="1"/>
+    <col min="110" max="110" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="111" max="111" width="15" bestFit="1" customWidth="1"/>
+    <col min="112" max="112" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="113" max="113" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="114" max="114" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="115" max="115" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="116" max="116" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="117" max="117" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="118" max="118" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="119" max="119" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="120" max="120" width="26.83203125" bestFit="1" customWidth="1"/>
+    <col min="121" max="121" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="122" max="122" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="123" max="123" width="45" bestFit="1" customWidth="1"/>
+    <col min="124" max="124" width="24.1640625" bestFit="1" customWidth="1"/>
+    <col min="125" max="125" width="22.83203125" bestFit="1" customWidth="1"/>
+    <col min="126" max="126" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="127" max="127" width="17" bestFit="1" customWidth="1"/>
+    <col min="128" max="128" width="18" bestFit="1" customWidth="1"/>
+    <col min="129" max="129" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="130" max="130" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="131" max="131" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="132" max="132" width="22.5" bestFit="1" customWidth="1"/>
+    <col min="133" max="133" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="134" max="134" width="24.83203125" bestFit="1" customWidth="1"/>
+    <col min="135" max="135" width="25.5" bestFit="1" customWidth="1"/>
+    <col min="136" max="136" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="137" max="137" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="138" max="138" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="139" max="139" width="42.33203125" bestFit="1" customWidth="1"/>
+    <col min="140" max="140" width="28.6640625" bestFit="1" customWidth="1"/>
+    <col min="141" max="142" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="143" max="143" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="144" max="144" width="34.5" bestFit="1" customWidth="1"/>
+    <col min="145" max="145" width="34" bestFit="1" customWidth="1"/>
+    <col min="146" max="146" width="36.5" bestFit="1" customWidth="1"/>
+    <col min="147" max="147" width="37" bestFit="1" customWidth="1"/>
+    <col min="148" max="148" width="35.83203125" bestFit="1" customWidth="1"/>
+    <col min="149" max="149" width="28.1640625" bestFit="1" customWidth="1"/>
+    <col min="150" max="150" width="30.5" bestFit="1" customWidth="1"/>
+    <col min="151" max="151" width="31" bestFit="1" customWidth="1"/>
+    <col min="152" max="152" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="153" max="153" width="42.33203125" bestFit="1" customWidth="1"/>
+    <col min="154" max="154" width="35.5" bestFit="1" customWidth="1"/>
+    <col min="155" max="155" width="39" bestFit="1" customWidth="1"/>
+    <col min="156" max="156" width="38.5" bestFit="1" customWidth="1"/>
+    <col min="157" max="157" width="41" bestFit="1" customWidth="1"/>
+    <col min="158" max="158" width="41.33203125" bestFit="1" customWidth="1"/>
+    <col min="159" max="159" width="40.33203125" bestFit="1" customWidth="1"/>
+    <col min="160" max="160" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="161" max="161" width="28.1640625" bestFit="1" customWidth="1"/>
+    <col min="162" max="162" width="28.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:162" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -8610,9 +8776,175 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:FF16"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="30.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="29.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="29.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="3.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="42.33203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="21" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="18" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="16" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="24" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="16" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="20" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="22" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="19" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="20" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="22.5" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="25.5" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="19" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="21.1640625" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="23" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="25.1640625" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="22" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="25.1640625" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="24" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="21.1640625" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="24.5" bestFit="1" customWidth="1"/>
+    <col min="76" max="76" width="24.83203125" bestFit="1" customWidth="1"/>
+    <col min="77" max="77" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="78" max="78" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="79" max="79" width="24" bestFit="1" customWidth="1"/>
+    <col min="80" max="80" width="21.83203125" bestFit="1" customWidth="1"/>
+    <col min="81" max="81" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="82" max="82" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="83" max="83" width="25" bestFit="1" customWidth="1"/>
+    <col min="84" max="84" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="85" max="85" width="28.1640625" bestFit="1" customWidth="1"/>
+    <col min="86" max="86" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="87" max="87" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="88" max="88" width="23.83203125" bestFit="1" customWidth="1"/>
+    <col min="89" max="89" width="25.5" bestFit="1" customWidth="1"/>
+    <col min="90" max="90" width="22.5" bestFit="1" customWidth="1"/>
+    <col min="91" max="91" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="92" max="92" width="27.83203125" bestFit="1" customWidth="1"/>
+    <col min="93" max="93" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="94" max="94" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="95" max="95" width="20" bestFit="1" customWidth="1"/>
+    <col min="96" max="96" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="97" max="97" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="98" max="98" width="17" bestFit="1" customWidth="1"/>
+    <col min="99" max="99" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="100" max="100" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="101" max="101" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="102" max="102" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="103" max="103" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="104" max="104" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="105" max="105" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="106" max="106" width="15" bestFit="1" customWidth="1"/>
+    <col min="107" max="107" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="108" max="108" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="109" max="109" width="23" bestFit="1" customWidth="1"/>
+    <col min="110" max="110" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="111" max="111" width="15" bestFit="1" customWidth="1"/>
+    <col min="112" max="112" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="113" max="113" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="114" max="114" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="115" max="115" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="116" max="116" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="117" max="117" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="118" max="118" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="119" max="119" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="120" max="120" width="26.83203125" bestFit="1" customWidth="1"/>
+    <col min="121" max="121" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="122" max="122" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="123" max="123" width="45" bestFit="1" customWidth="1"/>
+    <col min="124" max="124" width="24.1640625" bestFit="1" customWidth="1"/>
+    <col min="125" max="125" width="22.83203125" bestFit="1" customWidth="1"/>
+    <col min="126" max="126" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="127" max="127" width="17" bestFit="1" customWidth="1"/>
+    <col min="128" max="128" width="18" bestFit="1" customWidth="1"/>
+    <col min="129" max="129" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="130" max="130" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="131" max="131" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="132" max="132" width="22.5" bestFit="1" customWidth="1"/>
+    <col min="133" max="133" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="134" max="134" width="24.83203125" bestFit="1" customWidth="1"/>
+    <col min="135" max="135" width="25.5" bestFit="1" customWidth="1"/>
+    <col min="136" max="136" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="137" max="137" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="138" max="138" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="139" max="139" width="42.33203125" bestFit="1" customWidth="1"/>
+    <col min="140" max="140" width="28.6640625" bestFit="1" customWidth="1"/>
+    <col min="141" max="141" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="142" max="142" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="143" max="143" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="144" max="144" width="34.5" bestFit="1" customWidth="1"/>
+    <col min="145" max="145" width="34" bestFit="1" customWidth="1"/>
+    <col min="146" max="146" width="36.5" bestFit="1" customWidth="1"/>
+    <col min="147" max="147" width="37" bestFit="1" customWidth="1"/>
+    <col min="148" max="148" width="35.83203125" bestFit="1" customWidth="1"/>
+    <col min="149" max="149" width="28.1640625" bestFit="1" customWidth="1"/>
+    <col min="150" max="150" width="30.5" bestFit="1" customWidth="1"/>
+    <col min="151" max="151" width="31" bestFit="1" customWidth="1"/>
+    <col min="152" max="152" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="153" max="153" width="42.33203125" bestFit="1" customWidth="1"/>
+    <col min="154" max="154" width="35.5" bestFit="1" customWidth="1"/>
+    <col min="155" max="155" width="39" bestFit="1" customWidth="1"/>
+    <col min="156" max="156" width="38.5" bestFit="1" customWidth="1"/>
+    <col min="157" max="157" width="41" bestFit="1" customWidth="1"/>
+    <col min="158" max="158" width="41.33203125" bestFit="1" customWidth="1"/>
+    <col min="159" max="159" width="40.33203125" bestFit="1" customWidth="1"/>
+    <col min="160" max="160" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="161" max="161" width="28.1640625" bestFit="1" customWidth="1"/>
+    <col min="162" max="162" width="28.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:162" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -12386,5 +12718,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>